<commit_message>
More update to topic
</commit_message>
<xml_diff>
--- a/2023-11-30 topic areas.xlsx
+++ b/2023-11-30 topic areas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA9DE61-F590-40EC-AC3A-3FB7AB9F1225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75CED64-E4E9-4B25-A6DA-F11782DB2FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="15180" windowHeight="19370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="15520" windowHeight="19370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>4. Surveillance of infection. This section outlines the principles and purpose of surveillance. It encompasses monitoring individual infection statuses and elucidates strategies for effective outbreak management.</t>
   </si>
   <si>
-    <t>7. Strategies for healthcare settings. This section covers education focusing on risk assessment and proper PPE usage for CF patients, healthcare professionals in hospitals and the community, and involvement of family and friends. It emphasizes hand hygiene, environmental cleaning, and disinfection, including water safety, ventilation quality, room, and equipment disinfection, along with specific protocols for pulmonary function testing areas. It also discusses auditing, the patient journey in hospitals (cohort vs. individual segregation, movement, and healthcare activities), and considerations during construction and renovation work within healthcare facilities.</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.  Routes of transmission.  This section includes contact transmission, respiratory pathways (including droplet and airborne transmission) and includes challenges regarding the current evidence of the literature. </t>
   </si>
   <si>
@@ -48,7 +45,10 @@
     <t xml:space="preserve">10. Future research recommendations.  This includes thoughts for future research ideas, and in particular also discusses infection prevention and control in an era of cystic fibrosis transmembrane receptor modulator drugs.  </t>
   </si>
   <si>
-    <t>6. Strategies to reduce transmission and acquisition in healthcare settings. This section encompasses approaches such as education, emphasizing risk assessment, and proper usage of personal protective equipment (PPE, such as gloves, aprons, face masks) for cystic fibrosis (CF) patients and / or healthcare professionals both within hospital premises and in the community, and the involvement of family and friends. It considers hand hygiene and  environmental cleaning and disinfection within hospitals.  It includes  water safety, ventilation quality, disinfection protocols for rooms and equipment, and specific considerations for pulmonary function testing areas involving negative pressure rooms, HEPA filters, timing between patients, and UV germicidal irradiation.  Audit of infection control is also considered.</t>
+    <t>6. Strategies to reduce transmission and acquisition in healthcare settings. This section encompasses approaches such as education, emphasizing risk assessment, and  usage of personal protective equipment (PPE, such as gloves, aprons, face masks) for cystic fibrosis (CF) patients and / or healthcare professionals both within hospital premises and in the community, and the involvement of family and friends. It considers hand hygiene and  environmental cleaning and disinfection within hospitals.  It includes  water safety, ventilation quality, disinfection protocols for rooms and equipment, and specific considerations for pulmonary function testing areas involving negative pressure rooms, HEPA filters, timing between patients, and UV germicidal irradiation.  Audit of infection control is also considered.</t>
+  </si>
+  <si>
+    <t>7. Strategies for non-healthcare settings. This section covers various domains including home, indoor settings, gyms, outdoor environments, educational settings from pre-school to higher education, and travel considerations. It emphasizes strategies like cleaning rooms and equipment, ensuring water safety, addressing potential risks in outdoor activities, and implementing preventive measures in educational settings and during travel, especially air travel. Additionally, it highlights the importance of viral transmission prevention and immunization against diseases such as flu, COVID-19, RSV, and pneumococcus, aligning with considerations in the CF Trust Antibiotic Treatment guideline.</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -425,27 +425,27 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>